<commit_message>
todos os tweets classificados
</commit_message>
<xml_diff>
--- a/tweets_riot.xlsx
+++ b/tweets_riot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaa\Documents\GitHub\projeto2_CD2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D0C0221-E6B2-4C61-9D64-1040B8B7871E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86301CA5-8DF4-45B9-805D-75AD08BF1504}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2007,8 +2007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A294" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B302" sqref="B302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
@@ -2515,1214 +2515,1937 @@
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>61</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B298">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="2"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="2"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>